<commit_message>
ASGEO2_REAL1_4 restart + ASGEO2_REAL2_1 + tuning P std1 s + soma Ackley
</commit_message>
<xml_diff>
--- a/ExecucoesGerais/ex_porcentagem_tunado.xlsx
+++ b/ExecucoesGerais/ex_porcentagem_tunado.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14460" windowHeight="7965" activeTab="5"/>
+    <workbookView windowWidth="19485" windowHeight="7965" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="GRI" sheetId="1" r:id="rId1"/>
@@ -35,15 +35,47 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -65,22 +97,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -93,16 +110,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -112,6 +128,14 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -156,36 +180,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -202,31 +202,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -238,7 +226,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -262,7 +268,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -274,25 +304,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -304,85 +382,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -393,15 +393,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -424,7 +415,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -440,6 +431,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -498,148 +498,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -21253,8 +21253,8 @@
   <sheetPr/>
   <dimension ref="A1:C201"/>
   <sheetViews>
-    <sheetView topLeftCell="A181" workbookViewId="0">
-      <selection activeCell="L187" sqref="L187"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A201" sqref="A2:A201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="2"/>
@@ -23485,8 +23485,8 @@
   <sheetPr/>
   <dimension ref="A1:C201"/>
   <sheetViews>
-    <sheetView topLeftCell="A186" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:C201"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C201" sqref="C1:C201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="2"/>
@@ -25717,8 +25717,8 @@
   <sheetPr/>
   <dimension ref="A1:C201"/>
   <sheetViews>
-    <sheetView topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:C201"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C201" sqref="C2:C201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="2"/>
@@ -27949,8 +27949,8 @@
   <sheetPr/>
   <dimension ref="A1:C201"/>
   <sheetViews>
-    <sheetView topLeftCell="A183" workbookViewId="0">
-      <selection activeCell="D201" sqref="D201"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C201" sqref="C2:C201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="2"/>
@@ -30181,8 +30181,8 @@
   <sheetPr/>
   <dimension ref="A1:C201"/>
   <sheetViews>
-    <sheetView topLeftCell="A183" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C201" sqref="C2:C201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="2"/>
@@ -32413,8 +32413,8 @@
   <sheetPr/>
   <dimension ref="A1:C201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
-      <selection activeCell="F189" sqref="F189"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C201" sqref="C2:C201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="2"/>

</xml_diff>